<commit_message>
[Justice Counts] Add the rest of the Metricfile definitions (Recidiviz/recidiviz-data#14697)
GitOrigin-RevId: e229962795a0c586dfb64d0836c247abb96d5d6b
</commit_message>
<xml_diff>
--- a/recidiviz/tests/justice_counts/bulk_upload/bulk_upload_fixtures/prosecution/prosecution_metrics.xlsx
+++ b/recidiviz/tests/justice_counts/bulk_upload/bulk_upload_fixtures/prosecution/prosecution_metrics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lilidworkin/recidiviz/recidiviz-data/recidiviz/tests/justice_counts/bulk_upload/bulk_upload_fixtures/prosecution/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E73EB27-30D5-DD4E-BBC5-9FC13704522A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{505B6EF4-5F8B-794D-B757-D7D448B2A72B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="49160" yWindow="1760" windowWidth="23300" windowHeight="17600" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="44140" yWindow="2120" windowWidth="23300" windowHeight="17600" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="caseloads" sheetId="12" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="cases_referred_by_severity" sheetId="15" r:id="rId4"/>
     <sheet name="cases_referred" sheetId="16" r:id="rId5"/>
     <sheet name="cases_rejected_by_gender" sheetId="17" r:id="rId6"/>
-    <sheet name="cases_rejected_by_raceethnicity" sheetId="18" r:id="rId7"/>
+    <sheet name="cases_rejected_by_race" sheetId="18" r:id="rId7"/>
     <sheet name="cases_rejected_by_severity" sheetId="19" r:id="rId8"/>
     <sheet name="cases_rejected" sheetId="20" r:id="rId9"/>
     <sheet name="violations_filed" sheetId="21" r:id="rId10"/>
@@ -37,7 +37,7 @@
     <definedName name="cases_referred_by_severity" localSheetId="3">cases_referred_by_severity!$A$1:$D$4</definedName>
     <definedName name="cases_rejected" localSheetId="8">cases_rejected!$A$1:$C$4</definedName>
     <definedName name="cases_rejected_by_gender" localSheetId="5">cases_rejected_by_gender!$A$1:$D$4</definedName>
-    <definedName name="cases_rejected_by_raceethnicity" localSheetId="6">cases_rejected_by_raceethnicity!$A$1:$D$4</definedName>
+    <definedName name="cases_rejected_by_raceethnicity" localSheetId="6">cases_rejected_by_race!$A$1:$D$4</definedName>
     <definedName name="cases_rejected_by_severity" localSheetId="7">cases_rejected_by_severity!$A$1:$D$4</definedName>
     <definedName name="total_staff_by_type" localSheetId="12">total_staff_by_type!$A$1:$C$4</definedName>
     <definedName name="violations_filed" localSheetId="9">violations_filed!$A$1:$B$3</definedName>
@@ -49,7 +49,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
   <connection id="1" xr16:uid="{3B67DEB5-A461-1643-AD1C-FFDE40D2397D}" name="caseloads" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/lilidworkin/recidiviz/recidiviz-data/recidiviz/tests/justice_counts/bulk_upload/bulk_upload_fixtures/prosecution/caseloads.csv" comma="1">
+    <textPr sourceFile="/Users/lilidworkin/recidiviz/recidiviz-data/recidiviz/tests/justice_counts/bulk_upload/bulk_upload_fixtures/prosecution/caseloads.csv" comma="1">
       <textFields count="3">
         <textField/>
         <textField/>
@@ -58,7 +58,7 @@
     </textPr>
   </connection>
   <connection id="2" xr16:uid="{68219654-06E7-5343-92C2-2636C8BCDC14}" name="caseloads_by_severity" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/lilidworkin/recidiviz/recidiviz-data/recidiviz/tests/justice_counts/bulk_upload/bulk_upload_fixtures/prosecution/caseloads_by_severity.csv" comma="1">
+    <textPr sourceFile="/Users/lilidworkin/recidiviz/recidiviz-data/recidiviz/tests/justice_counts/bulk_upload/bulk_upload_fixtures/prosecution/caseloads_by_severity.csv" comma="1">
       <textFields count="4">
         <textField/>
         <textField/>
@@ -68,7 +68,7 @@
     </textPr>
   </connection>
   <connection id="3" xr16:uid="{BBC53FBA-310B-3040-BBD6-3FF481889F82}" name="cases_disposed" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/lilidworkin/recidiviz/recidiviz-data/recidiviz/tests/justice_counts/bulk_upload/bulk_upload_fixtures/prosecution/cases_disposed.csv" comma="1">
+    <textPr sourceFile="/Users/lilidworkin/recidiviz/recidiviz-data/recidiviz/tests/justice_counts/bulk_upload/bulk_upload_fixtures/prosecution/cases_disposed.csv" comma="1">
       <textFields count="3">
         <textField/>
         <textField/>
@@ -77,7 +77,7 @@
     </textPr>
   </connection>
   <connection id="4" xr16:uid="{CFF13463-254C-4249-BCB9-CA9B7D1C1F70}" name="cases_disposed_by_type" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/lilidworkin/recidiviz/recidiviz-data/recidiviz/tests/justice_counts/bulk_upload/bulk_upload_fixtures/prosecution/cases_disposed_by_type.csv" comma="1">
+    <textPr sourceFile="/Users/lilidworkin/recidiviz/recidiviz-data/recidiviz/tests/justice_counts/bulk_upload/bulk_upload_fixtures/prosecution/cases_disposed_by_type.csv" comma="1">
       <textFields count="4">
         <textField/>
         <textField/>
@@ -87,7 +87,7 @@
     </textPr>
   </connection>
   <connection id="5" xr16:uid="{EDDE3FCE-0785-6F43-BFE3-13BAC8322196}" name="cases_referred" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/lilidworkin/recidiviz/recidiviz-data/recidiviz/tests/justice_counts/bulk_upload/bulk_upload_fixtures/prosecution/cases_referred.csv" comma="1">
+    <textPr sourceFile="/Users/lilidworkin/recidiviz/recidiviz-data/recidiviz/tests/justice_counts/bulk_upload/bulk_upload_fixtures/prosecution/cases_referred.csv" comma="1">
       <textFields count="3">
         <textField/>
         <textField/>
@@ -96,7 +96,7 @@
     </textPr>
   </connection>
   <connection id="6" xr16:uid="{A92237C1-120E-1D44-BBC4-5A41C328F5C4}" name="cases_referred_by_severity" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/lilidworkin/recidiviz/recidiviz-data/recidiviz/tests/justice_counts/bulk_upload/bulk_upload_fixtures/prosecution/cases_referred_by_severity.csv" comma="1">
+    <textPr sourceFile="/Users/lilidworkin/recidiviz/recidiviz-data/recidiviz/tests/justice_counts/bulk_upload/bulk_upload_fixtures/prosecution/cases_referred_by_severity.csv" comma="1">
       <textFields count="4">
         <textField/>
         <textField/>
@@ -106,7 +106,7 @@
     </textPr>
   </connection>
   <connection id="7" xr16:uid="{8A731E99-AFD6-AA42-B86F-16D66B364F93}" name="cases_rejected" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/lilidworkin/recidiviz/recidiviz-data/recidiviz/tests/justice_counts/bulk_upload/bulk_upload_fixtures/prosecution/cases_rejected.csv" comma="1">
+    <textPr sourceFile="/Users/lilidworkin/recidiviz/recidiviz-data/recidiviz/tests/justice_counts/bulk_upload/bulk_upload_fixtures/prosecution/cases_rejected.csv" comma="1">
       <textFields count="3">
         <textField/>
         <textField/>
@@ -115,7 +115,7 @@
     </textPr>
   </connection>
   <connection id="8" xr16:uid="{0520DC19-BE18-564C-843F-50639D5977CB}" name="cases_rejected_by_gender" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/lilidworkin/recidiviz/recidiviz-data/recidiviz/tests/justice_counts/bulk_upload/bulk_upload_fixtures/prosecution/cases_rejected_by_gender.csv" comma="1">
+    <textPr sourceFile="/Users/lilidworkin/recidiviz/recidiviz-data/recidiviz/tests/justice_counts/bulk_upload/bulk_upload_fixtures/prosecution/cases_rejected_by_gender.csv" comma="1">
       <textFields count="4">
         <textField/>
         <textField/>
@@ -125,7 +125,7 @@
     </textPr>
   </connection>
   <connection id="9" xr16:uid="{F50580E3-1A9C-B343-B559-BA1ED0F712F8}" name="cases_rejected_by_raceethnicity" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/lilidworkin/recidiviz/recidiviz-data/recidiviz/tests/justice_counts/bulk_upload/bulk_upload_fixtures/prosecution/cases_rejected_by_raceethnicity.csv" comma="1">
+    <textPr sourceFile="/Users/lilidworkin/recidiviz/recidiviz-data/recidiviz/tests/justice_counts/bulk_upload/bulk_upload_fixtures/prosecution/cases_rejected_by_raceethnicity.csv" comma="1">
       <textFields count="4">
         <textField/>
         <textField/>
@@ -135,7 +135,7 @@
     </textPr>
   </connection>
   <connection id="10" xr16:uid="{A0FB9839-0865-ED43-A687-43C1F66CA23B}" name="cases_rejected_by_severity" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/lilidworkin/recidiviz/recidiviz-data/recidiviz/tests/justice_counts/bulk_upload/bulk_upload_fixtures/prosecution/cases_rejected_by_severity.csv" comma="1">
+    <textPr sourceFile="/Users/lilidworkin/recidiviz/recidiviz-data/recidiviz/tests/justice_counts/bulk_upload/bulk_upload_fixtures/prosecution/cases_rejected_by_severity.csv" comma="1">
       <textFields count="4">
         <textField/>
         <textField/>
@@ -145,7 +145,7 @@
     </textPr>
   </connection>
   <connection id="11" xr16:uid="{3A4D52CA-DE9A-224B-B02C-219164493C26}" name="total_staff_by_type" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/lilidworkin/recidiviz/recidiviz-data/recidiviz/tests/justice_counts/bulk_upload/bulk_upload_fixtures/prosecution/total_staff_by_type.csv" comma="1">
+    <textPr sourceFile="/Users/lilidworkin/recidiviz/recidiviz-data/recidiviz/tests/justice_counts/bulk_upload/bulk_upload_fixtures/prosecution/total_staff_by_type.csv" comma="1">
       <textFields count="3">
         <textField/>
         <textField/>
@@ -154,7 +154,7 @@
     </textPr>
   </connection>
   <connection id="12" xr16:uid="{7D45AD1C-5AEE-9145-A586-26FDC7DE0551}" name="violations_filed" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/lilidworkin/recidiviz/recidiviz-data/recidiviz/tests/justice_counts/bulk_upload/bulk_upload_fixtures/prosecution/violations_filed.csv" comma="1">
+    <textPr sourceFile="/Users/lilidworkin/recidiviz/recidiviz-data/recidiviz/tests/justice_counts/bulk_upload/bulk_upload_fixtures/prosecution/violations_filed.csv" comma="1">
       <textFields count="2">
         <textField/>
         <textField/>
@@ -1606,7 +1606,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90596B8F-E1C7-3A48-A361-146A9D31501E}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -30441,7 +30441,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9150DA24-DDF0-5442-8038-95FDCC9EBE70}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>

</xml_diff>